<commit_message>
FUnction to update was added
</commit_message>
<xml_diff>
--- a/Aircrafts.xlsx
+++ b/Aircrafts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>rf56</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>RF12</t>
+  </si>
+  <si>
+    <t>RF32</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.88671875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="14.5546875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -468,13 +471,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>280.0</v>
+        <v>600.0</v>
       </c>
       <c r="C7" t="n">
-        <v>560.0</v>
+        <v>600.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Airport and Aircraft were finished, and now the program show option for type of aircraft, airport (both source and destination) in order to get all the information required and showing on the reports
</commit_message>
<xml_diff>
--- a/Aircrafts.xlsx
+++ b/Aircrafts.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\IdeaProjects\Projects\unit3-project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\IdeaProjects\Projects\unit3-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBB81CE-DD2C-441F-BFB8-8909180941F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9136A6DD-75DF-49D2-8B84-37AD57695152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>NO AIRCRAFT</t>
+  </si>
+  <si>
+    <t>MODEL</t>
+  </si>
+  <si>
+    <t>PASSENGER CAPACITY</t>
+  </si>
+  <si>
+    <t>FULL TANKS FULL</t>
+  </si>
   <si>
     <t>rf56</t>
   </si>
@@ -40,21 +52,6 @@
   </si>
   <si>
     <t>RF52</t>
-  </si>
-  <si>
-    <t>MODEL</t>
-  </si>
-  <si>
-    <t>PASSENGER CAPACITY</t>
-  </si>
-  <si>
-    <t>FULL TANKS FULL</t>
-  </si>
-  <si>
-    <t>RF44</t>
-  </si>
-  <si>
-    <t>RF12</t>
   </si>
   <si>
     <t>RF32</t>
@@ -64,7 +61,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,93 +387,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E1" sqref="E1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>300</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
       <c r="C2">
         <v>300</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="D2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>350</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
         <v>310</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>500</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
         <v>420</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>600</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="n">
-        <v>600.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>600.0</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+      <c r="D7">
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>